<commit_message>
Mise à jour Journal de travail
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail-DTZ_DMS.xlsx
+++ b/Documentation/JournalDeTravail-DTZ_DMS.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>Nom du Projet :</t>
   </si>
@@ -124,6 +124,27 @@
   </si>
   <si>
     <t>Mise à jour de l'IceScrum(Userstory, Sprint)</t>
+  </si>
+  <si>
+    <t>Choix Template</t>
+  </si>
+  <si>
+    <t>Choix d'un template E-Commerce pour le début du code</t>
+  </si>
+  <si>
+    <t>Recherche d'un template</t>
+  </si>
+  <si>
+    <t>Recherche d'un template pour le commencement du code</t>
+  </si>
+  <si>
+    <t>Simão Henriques da Silva , Marcos Valente da Silva , Diego Pinto Tomaz</t>
+  </si>
+  <si>
+    <t>Début du code</t>
+  </si>
+  <si>
+    <t>j'ai codé dans l'index.php, controller.php et model.php</t>
   </si>
 </sst>
 </file>
@@ -674,40 +695,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -734,7 +728,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -747,6 +768,24 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
@@ -918,24 +957,6 @@
         <left style="medium">
           <color indexed="64"/>
         </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -1052,25 +1073,25 @@
     <tableColumn id="1" name="Date" dataDxfId="13"/>
     <tableColumn id="2" name="Heure debut" dataDxfId="12"/>
     <tableColumn id="3" name="Heure fin" dataDxfId="11"/>
-    <tableColumn id="4" name="Durée" dataDxfId="10">
+    <tableColumn id="4" name="Durée" dataDxfId="0">
       <calculatedColumnFormula>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Emplacement" dataDxfId="9"/>
-    <tableColumn id="7" name="Tâches" dataDxfId="8"/>
-    <tableColumn id="8" name="Résumé du travail" dataDxfId="7"/>
-    <tableColumn id="5" name="Fait par " dataDxfId="6"/>
+    <tableColumn id="6" name="Emplacement" dataDxfId="10"/>
+    <tableColumn id="7" name="Tâches" dataDxfId="9"/>
+    <tableColumn id="8" name="Résumé du travail" dataDxfId="8"/>
+    <tableColumn id="5" name="Fait par " dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau7" displayName="Tableau7" ref="C3:E63" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau7" displayName="Tableau7" ref="C3:E63" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="C3:E63"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Date" dataDxfId="2"/>
-    <tableColumn id="2" name="Description" dataDxfId="1"/>
-    <tableColumn id="3" name="Vip" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="3"/>
+    <tableColumn id="2" name="Description" dataDxfId="2"/>
+    <tableColumn id="3" name="Vip" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1341,8 +1362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N9999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,27 +1385,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
     </row>
     <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.25">
       <c r="F2" s="17"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
     </row>
     <row r="3" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F3" s="18"/>
@@ -1392,14 +1413,14 @@
       <c r="H3" s="18"/>
     </row>
     <row r="4" spans="2:14" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="48" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="49"/>
+      <c r="E4" s="40"/>
       <c r="G4" s="20" t="s">
         <v>1</v>
       </c>
@@ -1426,14 +1447,14 @@
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="46" t="s">
+      <c r="C5" s="32"/>
+      <c r="D5" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="47"/>
+      <c r="E5" s="38"/>
       <c r="G5" s="4">
         <v>44957</v>
       </c>
@@ -1461,14 +1482,14 @@
       </c>
     </row>
     <row r="6" spans="2:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="44">
+      <c r="C6" s="32"/>
+      <c r="D6" s="35">
         <v>44957</v>
       </c>
-      <c r="E6" s="45"/>
+      <c r="E6" s="36"/>
       <c r="G6" s="4">
         <v>44957</v>
       </c>
@@ -1496,15 +1517,15 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="40">
+      <c r="C7" s="48"/>
+      <c r="D7" s="49">
         <f>SUM(Tableau1[Durée])</f>
-        <v>0.15555555555555589</v>
+        <v>0.29097222222222241</v>
       </c>
-      <c r="E7" s="41"/>
+      <c r="E7" s="50"/>
       <c r="G7" s="4">
         <v>44958</v>
       </c>
@@ -1558,76 +1579,132 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="16"/>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="31"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="6"/>
+      <c r="D9" s="42"/>
+      <c r="G9" s="4">
+        <v>44977</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.35416666666666669</v>
+      </c>
       <c r="J9" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
+        <v>2.083333333333337E-2</v>
       </c>
-      <c r="K9" s="7"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="6"/>
+      <c r="D10" s="44"/>
+      <c r="G10" s="4">
+        <v>44978</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.70138888888888884</v>
+      </c>
       <c r="J10" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
+        <v>2.4305555555555469E-2</v>
       </c>
-      <c r="K10" s="7"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="35"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="6"/>
+      <c r="D11" s="46"/>
+      <c r="G11" s="4">
+        <v>44979</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="J11" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
+        <v>2.777777777777779E-2</v>
       </c>
-      <c r="K11" s="7"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="G12" s="4"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="6"/>
+      <c r="K11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="G12" s="4">
+        <v>44979</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.70138888888888884</v>
+      </c>
       <c r="J12" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
+        <v>6.2499999999999889E-2</v>
       </c>
-      <c r="K12" s="7"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+      <c r="K12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G13" s="4"/>
@@ -44162,18 +44239,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="G1:N2"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D4:E4"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1"/>
@@ -44534,9 +44611,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -44710,26 +44790,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D38AEF9-57C3-439A-B892-EB0F14AB4CC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE66B988-21FD-4E82-857E-C2E9A6618F3F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9b42e094-9454-4e38-a519-f9a276a20d04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -44753,9 +44822,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE66B988-21FD-4E82-857E-C2E9A6618F3F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D38AEF9-57C3-439A-B892-EB0F14AB4CC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9b42e094-9454-4e38-a519-f9a276a20d04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>